<commit_message>
Deploying to gh-pages from  @ fdf3c3bf2f226f87bce9e8f23c224819625077d7 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/4.b.1.1.xlsx
+++ b/en/downloads/data-excel/4.b.1.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>4.b.1.1 Расмий өкмөттөрдүн жана мамлекеттердин официалдык келишимдердин жана макулдашуулардын кабыл алуучу мамлекеттердин эсебинен кадрларды чет өлкөлордө даярдоо үчүн Кыргызстанга берилген орундардын саны*</t>
   </si>
@@ -506,9 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,7 +518,7 @@
     <col min="4" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +535,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -550,7 +552,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -561,8 +563,9 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -593,8 +596,11 @@
       <c r="J4" s="6">
         <v>2020</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -625,8 +631,11 @@
       <c r="J5" s="2">
         <v>370</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -657,8 +666,11 @@
       <c r="J6" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -689,8 +701,11 @@
       <c r="J7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -721,8 +736,11 @@
       <c r="J8" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -753,8 +771,11 @@
       <c r="J9" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -785,8 +806,11 @@
       <c r="J10" s="4">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>